<commit_message>
ExhibitF Word and Excel
Created Separate word files for each task Each word needs to be filled in. Also created an excel to keep track of progress in finishing off exhibit F
</commit_message>
<xml_diff>
--- a/AAG/ToDo/RFP 304404 ToDo.xlsx
+++ b/AAG/ToDo/RFP 304404 ToDo.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D4D2CFD-652A-4D81-A546-9A22AF1C1E82}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0076075-A422-4878-805A-64A42FD67ADB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t>#</t>
   </si>
@@ -85,6 +85,36 @@
   </si>
   <si>
     <t>\CFMTA Docs\"Questions_and_Answers_#1.pdf". Read.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compilation of word files for Exhibit F </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Simple Twitter App </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Look into Facebook Graph API Access </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GitHub - organize </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mihir + Nikhil </t>
+  </si>
+  <si>
+    <t>Analysis of tools available (Cost/Adv/Disadv/Reliability etc)</t>
+  </si>
+  <si>
+    <t>Mihir</t>
+  </si>
+  <si>
+    <t>Sangeeta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mihir </t>
+  </si>
+  <si>
+    <t xml:space="preserve">All </t>
   </si>
 </sst>
 </file>
@@ -482,7 +512,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -611,41 +641,71 @@
       <c r="A10" s="2">
         <v>7</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
+      <c r="B10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="3">
+        <v>43326</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2">
         <v>8</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
+      <c r="B11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="3">
+        <v>43326</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="2">
         <v>9</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
+      <c r="B12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="3">
+        <v>43326</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="2">
         <v>10</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
+      <c r="B13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="3">
+        <v>43326</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="2">
         <v>11</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
+      <c r="B14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="3">
+        <v>43326</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="2">

</xml_diff>